<commit_message>
Fixing SAP2000 model for Bridge3d
</commit_message>
<xml_diff>
--- a/Test/Bridge 3d/SAP2000.xlsx
+++ b/Test/Bridge 3d/SAP2000.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ModalAnalysis-OpenSeespy\Test\Bridge 3D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ModalAnalysis-OpenSeespy\Test\Bridge 3d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442E66E6-B0EC-4D35-9F0A-4674D02853EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDE8195-7985-4D95-B25E-2C589FD22AA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{93E55D6C-6A52-4DBC-A756-87119C251F67}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EEE2AAF-C1B1-4FB5-916E-6A8251E91FFE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Modal Load Participation Ratios" sheetId="1" r:id="rId1"/>
-    <sheet name="Modal Participating Mass Ratios" sheetId="2" r:id="rId2"/>
-    <sheet name="Modal Participation Factors" sheetId="3" r:id="rId3"/>
-    <sheet name="Modal Periods And Frequencies" sheetId="4" r:id="rId4"/>
-    <sheet name="Program Control" sheetId="5" r:id="rId5"/>
+    <sheet name="Assembled Joint Masses" sheetId="1" r:id="rId1"/>
+    <sheet name="Modal Load Participation Ratios" sheetId="2" r:id="rId2"/>
+    <sheet name="Modal Participating Mass Ratios" sheetId="3" r:id="rId3"/>
+    <sheet name="Modal Participation Factors" sheetId="4" r:id="rId4"/>
+    <sheet name="Modal Periods And Frequencies" sheetId="5" r:id="rId5"/>
+    <sheet name="Program Control" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="88">
+  <si>
+    <t>TABLE:  Assembled Joint Masses</t>
+  </si>
+  <si>
+    <t>Joint</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>KN-s2/m</t>
+  </si>
+  <si>
+    <t>KN-m-s2</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
   <si>
     <t>TABLE:  Modal Load Participation Ratios</t>
   </si>
@@ -49,9 +107,6 @@
     <t>Dynamic</t>
   </si>
   <si>
-    <t>Text</t>
-  </si>
-  <si>
     <t>Percent</t>
   </si>
   <si>
@@ -130,9 +185,6 @@
     <t>KN-s2</t>
   </si>
   <si>
-    <t>KN-m-s2</t>
-  </si>
-  <si>
     <t>KN-m</t>
   </si>
   <si>
@@ -239,15 +291,15 @@
   </si>
   <si>
     <t>AASHTO LRFD 2007</t>
+  </si>
+  <si>
+    <t>Mtot_unrestrained</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -331,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -347,7 +399,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,12 +712,289 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E9DEC93-6246-484A-BFF3-A2ADB368ACAC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A75F87-5127-490D-860A-DA05B8685C8F}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>400</v>
+      </c>
+      <c r="C4">
+        <v>400</v>
+      </c>
+      <c r="D4">
+        <v>400</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>948</v>
+      </c>
+      <c r="C5">
+        <v>948</v>
+      </c>
+      <c r="D5">
+        <v>948</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>1016</v>
+      </c>
+      <c r="C6">
+        <v>1016</v>
+      </c>
+      <c r="D6">
+        <v>1016</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>932</v>
+      </c>
+      <c r="C7">
+        <v>932</v>
+      </c>
+      <c r="D7">
+        <v>932</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>400</v>
+      </c>
+      <c r="C8">
+        <v>400</v>
+      </c>
+      <c r="D8">
+        <v>400</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>48</v>
+      </c>
+      <c r="C9">
+        <v>48</v>
+      </c>
+      <c r="D9">
+        <v>48</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>32</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12">
+        <f>SUM(B4:B8)</f>
+        <v>3696</v>
+      </c>
+      <c r="C12">
+        <f>SUM(C5:C7)</f>
+        <v>2896</v>
+      </c>
+      <c r="D12">
+        <f>SUM(D5:D7)</f>
+        <v>2896</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29731D7-902F-4C49-9852-8D7CBCD89A52}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection activeCell="I38" sqref="I38:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +1006,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -687,47 +1015,47 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>100</v>
@@ -738,13 +1066,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>100</v>
@@ -755,13 +1083,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>100</v>
@@ -772,31 +1100,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A39531-E581-45E3-874F-A48A59BD6DBA}">
-  <dimension ref="A1:P21"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FEF934-E869-4E84-AAC2-D86490C28B9A}">
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="9.140625" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.140625" customWidth="1"/>
@@ -804,7 +1128,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -824,110 +1148,110 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -974,10 +1298,10 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1024,10 +1348,10 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1074,10 +1398,10 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -1124,10 +1448,10 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -1174,10 +1498,10 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -1224,10 +1548,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -1274,10 +1598,10 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C11">
         <v>8</v>
@@ -1324,10 +1648,10 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C12">
         <v>9</v>
@@ -1374,10 +1698,10 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -1422,65 +1746,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>4.0062E-2</v>
+      </c>
+      <c r="E14">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1.1409999999999999E-5</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>1.8700000000000001E-5</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A73D3B-CDA6-41C3-9770-6D54FE183C17}">
-  <dimension ref="A1:L13"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B37A2D-98B4-496A-987D-8976C542C147}">
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:G13"/>
+      <selection activeCell="M38" sqref="M38:N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1488,7 +1814,8 @@
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
     <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -1497,7 +1824,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1513,86 +1840,86 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1601,22 +1928,22 @@
         <v>0.348192</v>
       </c>
       <c r="E4">
-        <v>-8.8280000000000007E-15</v>
+        <v>1.141E-14</v>
       </c>
       <c r="F4">
-        <v>97.949365999999998</v>
+        <v>30.974309000000002</v>
       </c>
       <c r="G4">
-        <v>-1.1130000000000001E-14</v>
+        <v>-5.1730000000000002E-15</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>1.251E-12</v>
+        <v>7.6989999999999998E-13</v>
       </c>
       <c r="J4">
-        <v>3551.5906049999999</v>
+        <v>1123.1115629999999</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1627,10 +1954,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1639,22 +1966,22 @@
         <v>0.27130300000000002</v>
       </c>
       <c r="E5">
-        <v>-1.5650000000000001E-14</v>
+        <v>3.3440000000000001E-14</v>
       </c>
       <c r="F5">
-        <v>-120.317108</v>
+        <v>38.047609999999999</v>
       </c>
       <c r="G5">
-        <v>4.2139999999999998E-14</v>
+        <v>-1.243E-14</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>-3.9680000000000001E-12</v>
+        <v>1.386E-12</v>
       </c>
       <c r="J5">
-        <v>-15211.675800000001</v>
+        <v>4810.3542690000004</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -1665,10 +1992,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1677,22 +2004,22 @@
         <v>0.21179999999999999</v>
       </c>
       <c r="E6">
-        <v>-191.155711</v>
+        <v>60.448743</v>
       </c>
       <c r="F6">
-        <v>3.5670000000000001E-14</v>
+        <v>-4.6230000000000002E-14</v>
       </c>
       <c r="G6">
-        <v>-0.17952599999999999</v>
+        <v>5.6771000000000002E-2</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>-20.22316</v>
+        <v>6.3951250000000002</v>
       </c>
       <c r="J6">
-        <v>3.7830000000000003E-12</v>
+        <v>-4.5120000000000002E-12</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -1703,10 +2030,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -1715,22 +2042,22 @@
         <v>0.14102700000000001</v>
       </c>
       <c r="E7">
-        <v>-8.286E-14</v>
+        <v>6.9639999999999994E-14</v>
       </c>
       <c r="F7">
-        <v>-69.926500000000004</v>
+        <v>22.112701000000001</v>
       </c>
       <c r="G7">
-        <v>-1.8039999999999999E-13</v>
+        <v>-3.8420000000000002E-14</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>1.0609999999999999E-11</v>
+        <v>-9.0829999999999998E-13</v>
       </c>
       <c r="J7">
-        <v>-6010.5842000000002</v>
+        <v>1900.71361</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -1741,10 +2068,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -1753,22 +2080,22 @@
         <v>0.107349</v>
       </c>
       <c r="E8">
-        <v>-7.6912669999999999</v>
+        <v>2.4321920000000001</v>
       </c>
       <c r="F8">
-        <v>1.5369999999999999E-13</v>
+        <v>-7.5759999999999997E-14</v>
       </c>
       <c r="G8">
-        <v>-4.7463999999999999E-2</v>
+        <v>1.5009E-2</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>3.2713040000000002</v>
+        <v>-1.0344770000000001</v>
       </c>
       <c r="J8">
-        <v>1.28E-11</v>
+        <v>-6.5660000000000001E-12</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1779,10 +2106,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -1791,22 +2118,22 @@
         <v>6.8943000000000004E-2</v>
       </c>
       <c r="E9">
-        <v>-0.59472499999999995</v>
+        <v>0.18806899999999999</v>
       </c>
       <c r="F9">
-        <v>-8.059E-14</v>
+        <v>-4.3550000000000001E-14</v>
       </c>
       <c r="G9">
-        <v>97.365401000000006</v>
+        <v>-30.789643000000002</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>-3889.4396999999999</v>
+        <v>1229.948828</v>
       </c>
       <c r="J9">
-        <v>-7.1280000000000003E-12</v>
+        <v>-3.7579999999999999E-12</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1817,10 +2144,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -1829,22 +2156,22 @@
         <v>5.5869000000000002E-2</v>
       </c>
       <c r="E10">
-        <v>2.9394070000000001</v>
+        <v>-0.92952199999999996</v>
       </c>
       <c r="F10">
-        <v>2.5910000000000001E-15</v>
+        <v>-2.1439999999999999E-16</v>
       </c>
       <c r="G10">
-        <v>-95.380367000000007</v>
+        <v>30.161919999999999</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>13307.60427</v>
+        <v>-4208.2340000000004</v>
       </c>
       <c r="J10">
-        <v>6.6019999999999995E-13</v>
+        <v>-1.4450000000000001E-14</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1855,10 +2182,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C11">
         <v>8</v>
@@ -1867,22 +2194,22 @@
         <v>5.5093999999999997E-2</v>
       </c>
       <c r="E11">
-        <v>18.468630999999998</v>
+        <v>5.8402940000000001</v>
       </c>
       <c r="F11">
-        <v>5.7779999999999995E-14</v>
+        <v>-3.299E-14</v>
       </c>
       <c r="G11">
-        <v>16.778054000000001</v>
+        <v>5.3056859999999997</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>-2478.2818699999998</v>
+        <v>-783.70153800000003</v>
       </c>
       <c r="J11">
-        <v>5.6909999999999999E-12</v>
+        <v>-2.9799999999999998E-12</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -1893,10 +2220,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C12">
         <v>9</v>
@@ -1905,22 +2232,22 @@
         <v>4.1550999999999998E-2</v>
       </c>
       <c r="E12">
-        <v>-1.013379</v>
+        <v>-0.32045899999999999</v>
       </c>
       <c r="F12">
-        <v>-2.91E-15</v>
+        <v>-2.9649999999999999E-14</v>
       </c>
       <c r="G12">
-        <v>-5.0188269999999999</v>
+        <v>-1.5870919999999999</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>453.844491</v>
+        <v>143.51822999999999</v>
       </c>
       <c r="J12">
-        <v>7.1339999999999997E-13</v>
+        <v>-2.3490000000000002E-12</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1931,10 +2258,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -1943,28 +2270,66 @@
         <v>4.1244999999999997E-2</v>
       </c>
       <c r="E13">
-        <v>0.13064000000000001</v>
+        <v>4.1312000000000001E-2</v>
       </c>
       <c r="F13">
-        <v>-6.5789999999999998E-15</v>
+        <v>-8.7899999999999997E-15</v>
       </c>
       <c r="G13">
-        <v>-100.376828</v>
+        <v>-31.74194</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>9031.1911089999994</v>
+        <v>2855.9133889999998</v>
       </c>
       <c r="J13">
-        <v>-2.6070000000000001E-12</v>
+        <v>-1.1269999999999999E-12</v>
       </c>
       <c r="K13">
         <v>1</v>
       </c>
       <c r="L13">
         <v>23207.003280000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>4.0062E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.95971399999999996</v>
+      </c>
+      <c r="F14">
+        <v>4.6360000000000004E-15</v>
+      </c>
+      <c r="G14">
+        <v>0.18177599999999999</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>-22.888766</v>
+      </c>
+      <c r="J14">
+        <v>4.171E-14</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>24598.111649999999</v>
       </c>
     </row>
   </sheetData>
@@ -1972,13 +2337,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FDD536C-0EBE-41A2-854B-96E462062A93}">
-  <dimension ref="A1:G13"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412FCCF2-94C7-4C65-B7D6-E8919D6CE5ED}">
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1992,7 +2355,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2003,56 +2366,56 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2072,10 +2435,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -2095,10 +2458,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -2118,10 +2481,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -2141,10 +2504,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -2164,10 +2527,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -2187,10 +2550,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -2210,10 +2573,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C11">
         <v>8</v>
@@ -2233,10 +2596,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C12">
         <v>9</v>
@@ -2256,10 +2619,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -2275,6 +2638,29 @@
       </c>
       <c r="G13">
         <v>23207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>4.0062E-2</v>
+      </c>
+      <c r="E14">
+        <v>24.962</v>
+      </c>
+      <c r="F14">
+        <v>156.84</v>
+      </c>
+      <c r="G14">
+        <v>24598</v>
       </c>
     </row>
   </sheetData>
@@ -2282,8 +2668,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1FCC59-A665-436E-8EA8-C3EA0A151B81}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDFE238-CF83-406E-AE6A-16FBDF207004}">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2309,7 +2695,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2329,146 +2715,146 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="I4" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="J4" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="K4" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="L4" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="M4" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="N4" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="O4" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>